<commit_message>
Verification of physical data
</commit_message>
<xml_diff>
--- a/objectPixelLength.xlsx
+++ b/objectPixelLength.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margie\Documents\University\University\IE_YOS4\SEM2\Lab Project ELEN4002\NNDev\Solvability-SourceCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazi\Documents\LabProject\SourceCode\Solvability-SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34CC54A-56F8-47EA-9332-D994E93CFBE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B1101A-785D-4C35-A87E-5DD7B0C78E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Immanent" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="ProcessedData" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Immanent" sheetId="3" r:id="rId4"/>
+    <sheet name="originalData" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$I$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">originalData!$A$1:$I$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ProcessedData!$A$1:$N$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
   <si>
     <t>File</t>
   </si>
@@ -327,6 +330,21 @@
   </si>
   <si>
     <t>NNupperVolume</t>
+  </si>
+  <si>
+    <t>targetVolume</t>
+  </si>
+  <si>
+    <t>x_axis</t>
+  </si>
+  <si>
+    <t>y_axis</t>
+  </si>
+  <si>
+    <t>z_axis</t>
+  </si>
+  <si>
+    <t>NNOutput</t>
   </si>
 </sst>
 </file>
@@ -400,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -436,11 +454,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -508,6 +537,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,34 +820,709 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286D9129-FD4E-48F9-9A42-FC1E1BBAD9B8}">
-  <dimension ref="A1:R25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C899A52-F53E-4FF8-8981-E50601D65844}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="5">
+        <v>6.1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10.8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5">
+        <v>177.77538220187404</v>
+      </c>
+      <c r="H2" s="5">
+        <f>B2*C2*D2</f>
+        <v>395.28</v>
+      </c>
+      <c r="I2">
+        <v>379.88378381147328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C3" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D3" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>177.77548859229773</v>
+      </c>
+      <c r="H3" s="5">
+        <f>B3*C3*D3</f>
+        <v>132.65099999999998</v>
+      </c>
+      <c r="I3">
+        <v>150.64716194497203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5">
+        <v>177.77556838924232</v>
+      </c>
+      <c r="H4" s="5">
+        <f>PI()*D4*D4*(1/4)*B4</f>
+        <v>134.66593989245322</v>
+      </c>
+      <c r="I4">
+        <v>136.53034593418437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4.3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4.3</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4.3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>177.77574634923849</v>
+      </c>
+      <c r="H5" s="5">
+        <f>PI()*D5*D5*(1/4)*B5</f>
+        <v>62.444651777240921</v>
+      </c>
+      <c r="I5">
+        <v>53.143077134356489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="5">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>177.77553326696386</v>
+      </c>
+      <c r="H6" s="5">
+        <f>PI()*D6*D6*(1/4)*B6</f>
+        <v>311.01767270538954</v>
+      </c>
+      <c r="I6">
+        <v>257.17196238316836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>177.77591390441984</v>
+      </c>
+      <c r="H7" s="7">
+        <f>(4/3)*PI()*B7*C7*D8*(1/8)</f>
+        <v>109.32742434492479</v>
+      </c>
+      <c r="I7">
+        <v>123.6045804019755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="4">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
+        <v>177.77531977936928</v>
+      </c>
+      <c r="H8" s="5">
+        <f>B8*C8*D8</f>
+        <v>522</v>
+      </c>
+      <c r="I8">
+        <v>519.4574258631061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="C9" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="D9" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3</v>
+      </c>
+      <c r="G9" s="16">
+        <v>177.77582263484675</v>
+      </c>
+      <c r="H9" s="16">
+        <f>(1/3)*PI()*(D9/4)*D9*C9</f>
+        <v>20.814883925746969</v>
+      </c>
+      <c r="I9">
+        <v>26.951790622755919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>177.77594994429597</v>
+      </c>
+      <c r="H10" s="7">
+        <f>(4/3)*PI()*B10*C10*D11*(1/8)</f>
+        <v>130.89969389957471</v>
+      </c>
+      <c r="I10">
+        <v>93.152282007535192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>10</v>
+      </c>
+      <c r="E11" s="5">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>177.7754975448583</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ref="H11:H12" si="0">B11*C11*D11</f>
+        <v>94.5</v>
+      </c>
+      <c r="I11">
+        <v>96.413823158236809</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>177.77545252842538</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>226.98099999999994</v>
+      </c>
+      <c r="I12">
+        <v>231.79306493683993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="C13" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="E13" s="16">
+        <v>3</v>
+      </c>
+      <c r="F13" s="16">
+        <v>3</v>
+      </c>
+      <c r="G13" s="16">
+        <v>177.77565796097031</v>
+      </c>
+      <c r="H13" s="16">
+        <f>(1/3)*PI()*(D13/4)*D13*C13</f>
+        <v>75.234599068780568</v>
+      </c>
+      <c r="I13">
+        <v>74.36383934898565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="C14" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="D14" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>4</v>
+      </c>
+      <c r="F14" s="5">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5">
+        <v>177.77552104915992</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" ref="H14:H15" si="1">B14*C14*D14</f>
+        <v>74.088000000000008</v>
+      </c>
+      <c r="I14">
+        <v>72.230149364115107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7">
+        <v>6</v>
+      </c>
+      <c r="C15" s="7">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <v>177.77545613484017</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="I15">
+        <v>223.91034674678605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="16">
+        <v>4</v>
+      </c>
+      <c r="D16" s="16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>177.77598598096307</v>
+      </c>
+      <c r="H16" s="7">
+        <f>(4/3)*PI()*B16*C16*D17*(1/8)</f>
+        <v>33.510321638291124</v>
+      </c>
+      <c r="I16">
+        <v>42.86567759553138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
+        <v>177.77543474069375</v>
+      </c>
+      <c r="H17" s="5">
+        <f>B17*C17*D17</f>
+        <v>163.19999999999999</v>
+      </c>
+      <c r="I17">
+        <v>169.77066153506064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="6">
+        <v>26.3</v>
+      </c>
+      <c r="C18" s="6">
+        <v>26.3</v>
+      </c>
+      <c r="D18" s="6">
+        <v>4</v>
+      </c>
+      <c r="E18" s="5">
+        <v>4</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5">
+        <v>177.77508015193399</v>
+      </c>
+      <c r="H18" s="5">
+        <f>PI()*D18*D18*(1/4)*B18</f>
+        <v>330.49554715764623</v>
+      </c>
+      <c r="I18">
+        <v>330.66077880899815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E19" s="5">
+        <v>4</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
+        <v>177.77544079328521</v>
+      </c>
+      <c r="H19" s="5">
+        <f>B19*C19*D19</f>
+        <v>94.248000000000005</v>
+      </c>
+      <c r="I19">
+        <v>93.39192970951477</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="E20" s="16">
+        <v>3</v>
+      </c>
+      <c r="F20" s="16">
+        <v>3</v>
+      </c>
+      <c r="G20" s="16">
+        <v>177.77563575571247</v>
+      </c>
+      <c r="H20" s="16">
+        <f>(1/3)*PI()*(D20/4)*D20*C20</f>
+        <v>101.64204151669296</v>
+      </c>
+      <c r="I20">
+        <v>104.63603661855257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="C21" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="D21" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
+        <v>177.77597517031137</v>
+      </c>
+      <c r="H21" s="7">
+        <f>(4/3)*PI()*B21*C21*D22*(1/8)</f>
+        <v>38.725365443250176</v>
+      </c>
+      <c r="I21">
+        <v>59.883050178445963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="6">
+        <v>30.8</v>
+      </c>
+      <c r="C22" s="6">
+        <v>30.8</v>
+      </c>
+      <c r="D22" s="6">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5">
+        <v>4</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>177.7749435558635</v>
+      </c>
+      <c r="H22" s="5">
+        <f>PI()*D22*D22*(1/4)*B22</f>
+        <v>387.04421492226254</v>
+      </c>
+      <c r="I22">
+        <v>387.80391223027175</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H22" xr:uid="{EC738509-29E5-4558-A2F2-B02F01D847C0}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286D9129-FD4E-48F9-9A42-FC1E1BBAD9B8}">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="20.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
@@ -829,49 +1536,52 @@
         <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -884,59 +1594,63 @@
       <c r="D2" s="5">
         <v>6</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
+        <f>B2*C2*D2</f>
+        <v>395.28</v>
+      </c>
+      <c r="F2" s="4">
         <v>6.7114574704288543</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>11.870241960888947</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>7.2543649801799956</v>
       </c>
-      <c r="H2" s="14">
+      <c r="I2" s="14">
         <f>B2-(B2*0.14347)</f>
         <v>5.2248329999999994</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="14">
         <f>B2+(B2*0.14347)</f>
         <v>6.9751669999999999</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="14">
         <f>C2-(C2*0.14347)</f>
         <v>9.2505240000000004</v>
       </c>
-      <c r="K2" s="14">
+      <c r="L2" s="14">
         <f>C2+(C2*0.14347)</f>
         <v>12.349476000000001</v>
       </c>
-      <c r="L2" s="14">
+      <c r="M2" s="14">
         <f>D2-(D2*0.14347)</f>
         <v>5.1391799999999996</v>
       </c>
-      <c r="M2" s="14">
+      <c r="N2" s="14">
         <f>D2+(D2*0.14347)</f>
         <v>6.8608200000000004</v>
       </c>
-      <c r="N2" s="18">
-        <f>H2*J2*L2</f>
+      <c r="O2" s="18">
+        <f>I2*K2*M2</f>
         <v>248.38912473789762</v>
       </c>
-      <c r="O2" s="21">
-        <f>I2*K2*M2</f>
+      <c r="P2" s="21">
+        <f>J2*L2*N2</f>
         <v>590.98868471181447</v>
       </c>
-      <c r="P2" s="4">
-        <f>O2-N2</f>
+      <c r="Q2" s="4">
+        <f>P2-O2</f>
         <v>342.59955997391683</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="R2" s="18">
         <v>248.38707413832608</v>
       </c>
-      <c r="R2" s="21">
+      <c r="S2" s="21">
         <v>591.00014847088778</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>77</v>
       </c>
@@ -949,59 +1663,63 @@
       <c r="D3" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
+        <f>B3*C3*D3</f>
+        <v>132.65099999999998</v>
+      </c>
+      <c r="F3" s="4">
         <v>5.5996789821455</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>5.659121585663236</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>5.5192540947721325</v>
       </c>
-      <c r="H3" s="14">
-        <f t="shared" ref="H3:H22" si="0">B3-(B3*0.14347)</f>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I22" si="0">B3-(B3*0.14347)</f>
         <v>4.368303</v>
       </c>
-      <c r="I3" s="14">
-        <f t="shared" ref="I3:I22" si="1">B3+(B3*0.14347)</f>
+      <c r="J3" s="14">
+        <f t="shared" ref="J3:J22" si="1">B3+(B3*0.14347)</f>
         <v>5.8316969999999992</v>
       </c>
-      <c r="J3" s="14">
-        <f t="shared" ref="J3:J22" si="2">C3-(C3*0.14347)</f>
+      <c r="K3" s="14">
+        <f t="shared" ref="K3:K22" si="2">C3-(C3*0.14347)</f>
         <v>4.368303</v>
       </c>
-      <c r="K3" s="14">
-        <f t="shared" ref="K3:K22" si="3">C3+(C3*0.14347)</f>
+      <c r="L3" s="14">
+        <f t="shared" ref="L3:L22" si="3">C3+(C3*0.14347)</f>
         <v>5.8316969999999992</v>
       </c>
-      <c r="L3" s="14">
-        <f t="shared" ref="L3:L22" si="4">D3-(D3*0.14347)</f>
+      <c r="M3" s="14">
+        <f t="shared" ref="M3:M22" si="4">D3-(D3*0.14347)</f>
         <v>4.368303</v>
       </c>
-      <c r="M3" s="14">
-        <f t="shared" ref="M3:M22" si="5">D3+(D3*0.14347)</f>
+      <c r="N3" s="14">
+        <f t="shared" ref="N3:N22" si="5">D3+(D3*0.14347)</f>
         <v>5.8316969999999992</v>
       </c>
-      <c r="N3" s="18">
-        <f>H3*J3*L3</f>
+      <c r="O3" s="18">
+        <f>I3*K3*M3</f>
         <v>83.356268431508951</v>
       </c>
-      <c r="O3" s="21">
-        <f>I3*K3*M3</f>
+      <c r="P3" s="21">
+        <f>J3*L3*N3</f>
         <v>198.32837486264637</v>
       </c>
-      <c r="P3" s="4">
-        <f>O3-N3</f>
+      <c r="Q3" s="4">
+        <f>P3-O3</f>
         <v>114.97210643113742</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="R3" s="18">
         <v>83.357695799609402</v>
       </c>
-      <c r="R3" s="21">
+      <c r="S3" s="21">
         <v>198.32782964828547</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
@@ -1014,59 +1732,63 @@
       <c r="D4" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
+        <f>PI()*D4*D4*(1/4)*B4</f>
+        <v>134.66593989245322</v>
+      </c>
+      <c r="F4" s="4">
         <v>10.727138063931609</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>10.774531100422447</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>4.8710075241818629</v>
       </c>
-      <c r="H4" s="14">
+      <c r="I4" s="14">
         <f t="shared" si="0"/>
         <v>8.7366060000000001</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="14">
         <f t="shared" si="1"/>
         <v>11.663393999999998</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="14">
         <f t="shared" si="2"/>
         <v>8.7366060000000001</v>
       </c>
-      <c r="K4" s="14">
+      <c r="L4" s="14">
         <f t="shared" si="3"/>
         <v>11.663393999999998</v>
       </c>
-      <c r="L4" s="14">
+      <c r="M4" s="14">
         <f t="shared" si="4"/>
         <v>3.5117729999999998</v>
       </c>
-      <c r="M4" s="14">
+      <c r="N4" s="14">
         <f t="shared" si="5"/>
         <v>4.6882269999999995</v>
       </c>
-      <c r="N4" s="18">
-        <f>PI()*(L4/2)*H4</f>
-        <v>48.193566072156081</v>
-      </c>
-      <c r="O4" s="21">
-        <f>PI()*(M4/2)*I4</f>
-        <v>85.892146357756587</v>
-      </c>
-      <c r="P4" s="4">
-        <f>O4-N4</f>
-        <v>37.698580285600507</v>
-      </c>
-      <c r="Q4" s="18">
+      <c r="O4" s="18">
+        <f>PI()*(M4/2)*(M4/2)*I4</f>
+        <v>84.622432052956881</v>
+      </c>
+      <c r="P4" s="21">
+        <f>PI()*(N4/2)*(N4/2)*J4</f>
+        <v>201.34093982119305</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>P4-O4</f>
+        <v>116.71850776823617</v>
+      </c>
+      <c r="R4" s="18">
         <v>268.04720777002291</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="21">
         <v>637.76477248168339</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>79</v>
       </c>
@@ -1079,59 +1801,63 @@
       <c r="D5" s="9">
         <v>4.3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
+        <f>PI()*D5*D5*(1/4)*B5</f>
+        <v>62.444651777240921</v>
+      </c>
+      <c r="F5" s="4">
         <v>4.8966479657959097</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>4.878909699520416</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>4.529738751960406</v>
       </c>
-      <c r="H5" s="14">
+      <c r="I5" s="14">
         <f t="shared" si="0"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="14">
         <f t="shared" si="1"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <f t="shared" si="2"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="K5" s="14">
+      <c r="L5" s="14">
         <f t="shared" si="3"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="L5" s="14">
+      <c r="M5" s="14">
         <f t="shared" si="4"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="M5" s="14">
+      <c r="N5" s="14">
         <f t="shared" si="5"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="N5" s="18">
-        <f t="shared" ref="N5:N6" si="6">PI()*(L5/2)*H5</f>
-        <v>21.307963574226825</v>
-      </c>
-      <c r="O5" s="21">
-        <f t="shared" ref="O5:O6" si="7">PI()*(M5/2)*I5</f>
-        <v>37.975748114656135</v>
-      </c>
-      <c r="P5" s="4">
-        <f t="shared" ref="P5:P6" si="8">O5-N5</f>
-        <v>16.667784540429309</v>
-      </c>
-      <c r="Q5" s="18">
+      <c r="O5" s="18">
+        <f t="shared" ref="O5:O6" si="6">PI()*(M5/2)*(M5/2)*I5</f>
+        <v>39.239456586499877</v>
+      </c>
+      <c r="P5" s="21">
+        <f t="shared" ref="P5:P6" si="7">PI()*(N5/2)*(N5/2)*J5</f>
+        <v>93.361876697831562</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5:Q6" si="8">P5-O5</f>
+        <v>54.122420111331685</v>
+      </c>
+      <c r="R5" s="18">
         <v>49.965771271225705</v>
       </c>
-      <c r="R5" s="21">
+      <c r="S5" s="21">
         <v>118.87115491800894</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
@@ -1144,59 +1870,63 @@
       <c r="D6" s="5">
         <v>6</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
+        <f>PI()*D6*D6*(1/4)*B6</f>
+        <v>311.01767270538954</v>
+      </c>
+      <c r="F6" s="4">
         <v>12.677575544951022</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>12.733775774183615</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>7.4596040471631788</v>
       </c>
-      <c r="H6" s="14">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>9.4218299999999999</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="14">
         <f t="shared" si="1"/>
         <v>12.57817</v>
       </c>
-      <c r="J6" s="14">
+      <c r="K6" s="14">
         <f t="shared" si="2"/>
         <v>9.4218299999999999</v>
       </c>
-      <c r="K6" s="14">
+      <c r="L6" s="14">
         <f t="shared" si="3"/>
         <v>12.57817</v>
       </c>
-      <c r="L6" s="14">
+      <c r="M6" s="14">
         <f t="shared" si="4"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="M6" s="14">
+      <c r="N6" s="14">
         <f t="shared" si="5"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="N6" s="18">
+      <c r="O6" s="18">
         <f t="shared" si="6"/>
-        <v>76.058712595942154</v>
-      </c>
-      <c r="O6" s="21">
+        <v>195.43970729940702</v>
+      </c>
+      <c r="P6" s="21">
         <f t="shared" si="7"/>
-        <v>135.55431993333184</v>
-      </c>
-      <c r="P6" s="4">
+        <v>465.00689464250087</v>
+      </c>
+      <c r="Q6" s="4">
         <f t="shared" si="8"/>
-        <v>59.495607337389686</v>
-      </c>
-      <c r="Q6" s="18">
+        <v>269.56718734309385</v>
+      </c>
+      <c r="R6" s="18">
         <v>456.21776420699564</v>
       </c>
-      <c r="R6" s="21">
+      <c r="S6" s="21">
         <v>1085.4227419716947</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>80</v>
       </c>
@@ -1209,59 +1939,63 @@
       <c r="D7" s="7">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
+        <f>(4/3)*PI()*B7*C7*D8*(1/8)</f>
+        <v>109.32742434492479</v>
+      </c>
+      <c r="F7" s="4">
         <v>7.0088071656435176</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>7.0075302740231953</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>6.9897066655491482</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="14">
         <f t="shared" si="1"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="J7" s="14">
+      <c r="K7" s="14">
         <f t="shared" si="2"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="K7" s="14">
+      <c r="L7" s="14">
         <f t="shared" si="3"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="L7" s="14">
+      <c r="M7" s="14">
         <f t="shared" si="4"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="M7" s="14">
+      <c r="N7" s="14">
         <f t="shared" si="5"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="N7" s="18">
-        <f>(4/3)*(H7/2)*(H7/2)*(H7/2)*PI()</f>
+      <c r="O7" s="18">
+        <f>(4/3)*(I7/2)*(I7/2)*(I7/2)*PI()</f>
         <v>71.06898447251163</v>
       </c>
-      <c r="O7" s="21">
-        <f>(4/3)*PI()*(I7/2)*(I7/2)*(I7/2)</f>
+      <c r="P7" s="21">
+        <f>(4/3)*PI()*(J7/2)*(J7/2)*(J7/2)</f>
         <v>169.09341623363667</v>
       </c>
-      <c r="P7" s="4">
-        <f>O7-N7</f>
+      <c r="Q7" s="4">
+        <f>P7-O7</f>
         <v>98.024431761125044</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="R7" s="18">
         <v>135.73042130373233</v>
       </c>
-      <c r="R7" s="21">
+      <c r="S7" s="21">
         <v>322.94916024268025</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>78</v>
       </c>
@@ -1275,58 +2009,62 @@
         <v>5.8</v>
       </c>
       <c r="E8" s="5">
+        <f>B8*C8*D8</f>
+        <v>522</v>
+      </c>
+      <c r="F8" s="5">
         <v>16.964535643126382</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>7.7917182141969104</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>7.8303170887052316</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>12.847950000000001</v>
       </c>
-      <c r="I8" s="14">
+      <c r="J8" s="14">
         <f t="shared" si="1"/>
         <v>17.152049999999999</v>
       </c>
-      <c r="J8" s="14">
+      <c r="K8" s="14">
         <f t="shared" si="2"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="K8" s="14">
+      <c r="L8" s="14">
         <f t="shared" si="3"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="L8" s="14">
+      <c r="M8" s="14">
         <f t="shared" si="4"/>
         <v>4.9678740000000001</v>
       </c>
-      <c r="M8" s="14">
+      <c r="N8" s="14">
         <f t="shared" si="5"/>
         <v>6.6321259999999995</v>
       </c>
-      <c r="N8" s="18">
-        <f>H8*J8*L8</f>
+      <c r="O8" s="18">
+        <f>I8*K8*M8</f>
         <v>328.01842520032017</v>
       </c>
-      <c r="O8" s="21">
-        <f>I8*K8*M8</f>
+      <c r="P8" s="21">
+        <f>J8*L8*N8</f>
         <v>780.44953809847971</v>
       </c>
-      <c r="P8" s="4">
-        <f>O8-N8</f>
+      <c r="Q8" s="4">
+        <f>P8-O8</f>
         <v>452.43111289815954</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="R8" s="18">
         <v>328.01424668606666</v>
       </c>
-      <c r="R8" s="21">
+      <c r="S8" s="21">
         <v>780.45544395645709</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>81</v>
       </c>
@@ -1339,59 +2077,63 @@
       <c r="D9" s="16">
         <v>4.3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="16">
+        <f>(1/3)*PI()*(D9/4)*D9*C9</f>
+        <v>20.814883925746969</v>
+      </c>
+      <c r="F9" s="4">
         <v>4.6666920039007787</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>4.6906107742357488</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>4.302146119837718</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="I9" s="14">
+      <c r="J9" s="14">
         <f t="shared" si="1"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="J9" s="14">
+      <c r="K9" s="14">
         <f t="shared" si="2"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="K9" s="14">
+      <c r="L9" s="14">
         <f t="shared" si="3"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="L9" s="14">
+      <c r="M9" s="14">
         <f t="shared" si="4"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="M9" s="14">
+      <c r="N9" s="14">
         <f t="shared" si="5"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="N9" s="18">
-        <f>PI()*(L9/2)*(L9/2)*(J9/3)</f>
+      <c r="O9" s="18">
+        <f>PI()*(M9/2)*(M9/2)*(K9/3)</f>
         <v>13.079818862166626</v>
       </c>
-      <c r="O9" s="21">
-        <f>PI()*(M9/2)*(M9/2)*(K9/3)</f>
+      <c r="P9" s="21">
+        <f>PI()*(N9/2)*(N9/2)*(L9/3)</f>
         <v>31.120625565943858</v>
       </c>
-      <c r="P9" s="4">
-        <f>O9-N9</f>
+      <c r="Q9" s="4">
+        <f>P9-O9</f>
         <v>18.040806703777232</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="R9" s="18">
         <v>49.965771271225705</v>
       </c>
-      <c r="R9" s="21">
+      <c r="S9" s="21">
         <v>118.87115491800894</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>80</v>
       </c>
@@ -1404,59 +2146,63 @@
       <c r="D10" s="10">
         <v>5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="7">
+        <f>(4/3)*PI()*B10*C10*D11*(1/8)</f>
+        <v>130.89969389957471</v>
+      </c>
+      <c r="F10" s="4">
         <v>5.50380889323168</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>5.5044457066158312</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>5.5302322850855203</v>
       </c>
-      <c r="H10" s="14">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>4.2826500000000003</v>
       </c>
-      <c r="I10" s="14">
+      <c r="J10" s="14">
         <f t="shared" si="1"/>
         <v>5.7173499999999997</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K10" s="14">
         <f t="shared" si="2"/>
         <v>4.2826500000000003</v>
       </c>
-      <c r="K10" s="14">
+      <c r="L10" s="14">
         <f t="shared" si="3"/>
         <v>5.7173499999999997</v>
       </c>
-      <c r="L10" s="14">
+      <c r="M10" s="14">
         <f t="shared" si="4"/>
         <v>4.2826500000000003</v>
       </c>
-      <c r="M10" s="14">
+      <c r="N10" s="14">
         <f t="shared" si="5"/>
         <v>5.7173499999999997</v>
       </c>
-      <c r="N10" s="18">
-        <f>(4/3)*(H10/2)*(H10/2)*(H10/2)*PI()</f>
+      <c r="O10" s="18">
+        <f>(4/3)*(I10/2)*(I10/2)*(I10/2)*PI()</f>
         <v>41.127884532703511</v>
       </c>
-      <c r="O10" s="21">
-        <f>(4/3)*PI()*(I10/2)*(I10/2)*(I10/2)</f>
+      <c r="P10" s="21">
+        <f>(4/3)*PI()*(J10/2)*(J10/2)*(J10/2)</f>
         <v>97.854986246317495</v>
       </c>
-      <c r="P10" s="4">
-        <f>O10-N10</f>
+      <c r="Q10" s="4">
+        <f>P10-O10</f>
         <v>56.727101713613983</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="R10" s="18">
         <v>78.550344497632352</v>
       </c>
-      <c r="R10" s="21">
+      <c r="S10" s="21">
         <v>186.88835893787095</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
@@ -1469,59 +2215,63 @@
       <c r="D11" s="4">
         <v>10</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:E12" si="9">B11*C11*D11</f>
+        <v>94.5</v>
+      </c>
+      <c r="F11" s="4">
         <v>1.4783497371948668</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>6.7895883655684122</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>11.871406677354781</v>
       </c>
-      <c r="H11" s="14">
+      <c r="I11" s="14">
         <f t="shared" si="0"/>
         <v>1.2847949999999999</v>
       </c>
-      <c r="I11" s="14">
+      <c r="J11" s="14">
         <f t="shared" si="1"/>
         <v>1.7152050000000001</v>
       </c>
-      <c r="J11" s="14">
+      <c r="K11" s="14">
         <f t="shared" si="2"/>
         <v>5.3961389999999998</v>
       </c>
-      <c r="K11" s="14">
+      <c r="L11" s="14">
         <f t="shared" si="3"/>
         <v>7.2038609999999998</v>
       </c>
-      <c r="L11" s="14">
+      <c r="M11" s="14">
         <f t="shared" si="4"/>
         <v>8.5653000000000006</v>
       </c>
-      <c r="M11" s="14">
+      <c r="N11" s="14">
         <f t="shared" si="5"/>
         <v>11.434699999999999</v>
       </c>
-      <c r="N11" s="18">
-        <f t="shared" ref="N11:N12" si="9">H11*J11*L11</f>
+      <c r="O11" s="18">
+        <f t="shared" ref="O11:O12" si="10">I11*K11*M11</f>
         <v>59.382645941437275</v>
       </c>
-      <c r="O11" s="21">
-        <f t="shared" ref="O11:O12" si="10">I11*K11*M11</f>
+      <c r="P11" s="21">
+        <f t="shared" ref="P11:P12" si="11">J11*L11*N11</f>
         <v>141.28827844886271</v>
       </c>
-      <c r="P11" s="4">
-        <f t="shared" ref="P11:P12" si="11">O11-N11</f>
+      <c r="Q11" s="4">
+        <f t="shared" ref="Q11:Q12" si="12">P11-O11</f>
         <v>81.905632507425437</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="R11" s="18">
         <v>59.36920182315086</v>
       </c>
-      <c r="R11" s="21">
+      <c r="S11" s="21">
         <v>141.27980430022856</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>77</v>
       </c>
@@ -1534,59 +2284,63 @@
       <c r="D12" s="7">
         <v>6.1</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
+        <f t="shared" si="9"/>
+        <v>226.98099999999994</v>
+      </c>
+      <c r="F12" s="4">
         <v>6.5719635550770681</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>6.9012361304546284</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>6.7090956079675221</v>
       </c>
-      <c r="H12" s="14">
+      <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>5.2248329999999994</v>
       </c>
-      <c r="I12" s="14">
+      <c r="J12" s="14">
         <f t="shared" si="1"/>
         <v>6.9751669999999999</v>
       </c>
-      <c r="J12" s="14">
+      <c r="K12" s="14">
         <f t="shared" si="2"/>
         <v>5.2248329999999994</v>
       </c>
-      <c r="K12" s="14">
+      <c r="L12" s="14">
         <f t="shared" si="3"/>
         <v>6.9751669999999999</v>
       </c>
-      <c r="L12" s="14">
+      <c r="M12" s="14">
         <f t="shared" si="4"/>
         <v>5.2248329999999994</v>
       </c>
-      <c r="M12" s="14">
+      <c r="N12" s="14">
         <f t="shared" si="5"/>
         <v>6.9751669999999999</v>
       </c>
-      <c r="N12" s="18">
-        <f t="shared" si="9"/>
+      <c r="O12" s="18">
+        <f t="shared" si="10"/>
         <v>142.63208844903036</v>
       </c>
-      <c r="O12" s="21">
-        <f t="shared" si="10"/>
+      <c r="P12" s="21">
+        <f t="shared" si="11"/>
         <v>339.362483921707</v>
       </c>
-      <c r="P12" s="4">
-        <f t="shared" si="11"/>
+      <c r="Q12" s="4">
+        <f t="shared" si="12"/>
         <v>196.73039547267663</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="R12" s="18">
         <v>142.63066187963082</v>
       </c>
-      <c r="R12" s="21">
+      <c r="S12" s="21">
         <v>339.36754737243683</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
@@ -1599,59 +2353,63 @@
       <c r="D13" s="6">
         <v>5.5</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="16">
+        <f>(1/3)*PI()*(D13/4)*D13*C13</f>
+        <v>75.234599068780568</v>
+      </c>
+      <c r="F13" s="6">
         <v>11.291598940097117</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="6">
         <v>11.326712914531802</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <v>5.3943870888664849</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I13" s="15">
         <f t="shared" si="0"/>
         <v>8.1370350000000009</v>
       </c>
-      <c r="I13" s="15">
+      <c r="J13" s="15">
         <f t="shared" si="1"/>
         <v>10.862964999999999</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="15">
         <f t="shared" si="2"/>
         <v>8.1370350000000009</v>
       </c>
-      <c r="K13" s="15">
+      <c r="L13" s="15">
         <f t="shared" si="3"/>
         <v>10.862964999999999</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M13" s="15">
         <f t="shared" si="4"/>
         <v>4.710915</v>
       </c>
-      <c r="M13" s="15">
+      <c r="N13" s="15">
         <f t="shared" si="5"/>
         <v>6.289085</v>
       </c>
-      <c r="N13" s="18">
-        <f>PI()*(L13/2)*(L13/2)*(J13/3)</f>
+      <c r="O13" s="18">
+        <f>PI()*(M13/2)*(M13/2)*(K13/3)</f>
         <v>47.276503270342687</v>
       </c>
-      <c r="O13" s="21">
-        <f>PI()*(M13/2)*(M13/2)*(K13/3)</f>
+      <c r="P13" s="21">
+        <f>PI()*(N13/2)*(N13/2)*(L13/3)</f>
         <v>112.48430669014198</v>
       </c>
-      <c r="P13" s="4">
-        <f>O13-N13</f>
+      <c r="Q13" s="4">
+        <f>P13-O13</f>
         <v>65.207803419799291</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="R13" s="18">
         <v>311.92598385243309</v>
       </c>
-      <c r="R13" s="21">
+      <c r="S13" s="21">
         <v>742.12590435975665</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>77</v>
       </c>
@@ -1664,59 +2422,63 @@
       <c r="D14" s="16">
         <v>4.2</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
+        <f t="shared" ref="E14:E15" si="13">B14*C14*D14</f>
+        <v>74.088000000000008</v>
+      </c>
+      <c r="F14" s="4">
         <v>4.496117870466442</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>4.5413474310270461</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>4.7411773057122772</v>
       </c>
-      <c r="H14" s="14">
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>3.5974260000000005</v>
       </c>
-      <c r="I14" s="14">
+      <c r="J14" s="14">
         <f t="shared" si="1"/>
         <v>4.8025739999999999</v>
       </c>
-      <c r="J14" s="14">
+      <c r="K14" s="14">
         <f t="shared" si="2"/>
         <v>3.5974260000000005</v>
       </c>
-      <c r="K14" s="14">
+      <c r="L14" s="14">
         <f t="shared" si="3"/>
         <v>4.8025739999999999</v>
       </c>
-      <c r="L14" s="14">
+      <c r="M14" s="14">
         <f t="shared" si="4"/>
         <v>3.5974260000000005</v>
       </c>
-      <c r="M14" s="14">
+      <c r="N14" s="14">
         <f t="shared" si="5"/>
         <v>4.8025739999999999</v>
       </c>
-      <c r="N14" s="18">
-        <f t="shared" ref="N14:N15" si="12">H14*J14*L14</f>
+      <c r="O14" s="18">
+        <f t="shared" ref="O14:O15" si="14">I14*K14*M14</f>
         <v>46.55599441808684</v>
       </c>
-      <c r="O14" s="21">
-        <f t="shared" ref="O14:O15" si="13">I14*K14*M14</f>
+      <c r="P14" s="21">
+        <f t="shared" ref="P14:P15" si="15">J14*L14*N14</f>
         <v>110.77001030390838</v>
       </c>
-      <c r="P14" s="4">
-        <f t="shared" ref="P14:P15" si="14">O14-N14</f>
+      <c r="Q14" s="4">
+        <f t="shared" ref="Q14:Q15" si="16">P14-O14</f>
         <v>64.214015885821539</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="R14" s="18">
         <v>46.560745679756309</v>
       </c>
-      <c r="R14" s="21">
+      <c r="S14" s="21">
         <v>110.76949453070699</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>77</v>
       </c>
@@ -1729,59 +2491,63 @@
       <c r="D15" s="7">
         <v>6</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="5">
+        <f t="shared" si="13"/>
+        <v>216</v>
+      </c>
+      <c r="F15" s="4">
         <v>6.6607829881121585</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>7.0309838426329607</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>6.9065618468009564</v>
       </c>
-      <c r="H15" s="14">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="I15" s="14">
+      <c r="J15" s="14">
         <f t="shared" si="1"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="J15" s="14">
+      <c r="K15" s="14">
         <f t="shared" si="2"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="K15" s="14">
+      <c r="L15" s="14">
         <f t="shared" si="3"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="L15" s="14">
+      <c r="M15" s="14">
         <f t="shared" si="4"/>
         <v>5.1391799999999996</v>
       </c>
-      <c r="M15" s="14">
+      <c r="N15" s="14">
         <f t="shared" si="5"/>
         <v>6.8608200000000004</v>
       </c>
-      <c r="N15" s="18">
-        <f t="shared" si="12"/>
+      <c r="O15" s="18">
+        <f t="shared" si="14"/>
         <v>135.7317621518566</v>
       </c>
-      <c r="O15" s="21">
-        <f t="shared" si="13"/>
+      <c r="P15" s="21">
+        <f t="shared" si="15"/>
         <v>322.9446364545434</v>
       </c>
-      <c r="P15" s="4">
-        <f t="shared" si="14"/>
+      <c r="Q15" s="4">
+        <f t="shared" si="16"/>
         <v>187.2128743026868</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="R15" s="18">
         <v>135.73042130373233</v>
       </c>
-      <c r="R15" s="21">
+      <c r="S15" s="21">
         <v>322.94916024268025</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>80</v>
       </c>
@@ -1794,59 +2560,63 @@
       <c r="D16" s="16">
         <v>4</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="7">
+        <f>(4/3)*PI()*B16*C16*D17*(1/8)</f>
+        <v>33.510321638291124</v>
+      </c>
+      <c r="F16" s="4">
         <v>4.5369905386243401</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>4.5233812990578866</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>4.520775244689534</v>
       </c>
-      <c r="H16" s="14">
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="I16" s="14">
+      <c r="J16" s="14">
         <f t="shared" si="1"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="J16" s="14">
+      <c r="K16" s="14">
         <f t="shared" si="2"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="K16" s="14">
+      <c r="L16" s="14">
         <f t="shared" si="3"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="L16" s="14">
+      <c r="M16" s="14">
         <f t="shared" si="4"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="M16" s="14">
+      <c r="N16" s="14">
         <f t="shared" si="5"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="N16" s="18">
-        <f>(4/3)*(H16/2)*(H16/2)*(H16/2)*PI()</f>
+      <c r="O16" s="18">
+        <f>(4/3)*(I16/2)*(I16/2)*(I16/2)*PI()</f>
         <v>21.057476880744193</v>
       </c>
-      <c r="O16" s="21">
-        <f>(4/3)*PI()*(I16/2)*(I16/2)*(I16/2)</f>
+      <c r="P16" s="21">
+        <f>(4/3)*PI()*(J16/2)*(J16/2)*(J16/2)</f>
         <v>50.101752958114552</v>
       </c>
-      <c r="P16" s="4">
-        <f t="shared" ref="P16:P22" si="15">O16-N16</f>
+      <c r="Q16" s="4">
+        <f t="shared" ref="Q16:Q22" si="17">P16-O16</f>
         <v>29.044276077370359</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="R16" s="18">
         <v>40.221761442924098</v>
       </c>
-      <c r="R16" s="21">
+      <c r="S16" s="21">
         <v>95.687718961306956</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>78</v>
       </c>
@@ -1859,59 +2629,63 @@
       <c r="D17" s="5">
         <v>4</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="5">
+        <f>B17*C17*D17</f>
+        <v>163.19999999999999</v>
+      </c>
+      <c r="F17" s="4">
         <v>4.4883928323935605</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>10.878836719693362</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>4.9843568225340347</v>
       </c>
-      <c r="H17" s="14">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="I17" s="14">
+      <c r="J17" s="14">
         <f t="shared" si="1"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="J17" s="14">
+      <c r="K17" s="14">
         <f t="shared" si="2"/>
         <v>8.7366060000000001</v>
       </c>
-      <c r="K17" s="14">
+      <c r="L17" s="14">
         <f t="shared" si="3"/>
         <v>11.663393999999998</v>
       </c>
-      <c r="L17" s="14">
+      <c r="M17" s="14">
         <f t="shared" si="4"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="M17" s="14">
+      <c r="N17" s="14">
         <f t="shared" si="5"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="N17" s="18">
-        <f>H17*J17*L17</f>
+      <c r="O17" s="18">
+        <f>I17*K17*M17</f>
         <v>102.55288695918057</v>
       </c>
-      <c r="O17" s="21">
-        <f>I17*K17*M17</f>
+      <c r="P17" s="21">
+        <f>J17*L17*N17</f>
         <v>244.00261421009941</v>
       </c>
-      <c r="P17" s="4">
-        <f t="shared" si="15"/>
+      <c r="Q17" s="4">
+        <f t="shared" si="17"/>
         <v>141.44972725091884</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="R17" s="18">
         <v>102.52529150861194</v>
       </c>
-      <c r="R17" s="21">
+      <c r="S17" s="21">
         <v>244.0074120778597</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>79</v>
       </c>
@@ -1924,59 +2698,63 @@
       <c r="D18" s="6">
         <v>4</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
+        <f>PI()*D18*D18*(1/4)*B18</f>
+        <v>330.49554715764623</v>
+      </c>
+      <c r="F18" s="6">
         <v>27.538346372295624</v>
       </c>
-      <c r="F18" s="6">
+      <c r="G18" s="6">
         <v>27.580091548852078</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="6">
         <v>6.8833264817427562</v>
       </c>
-      <c r="H18" s="15">
+      <c r="I18" s="15">
         <f t="shared" si="0"/>
         <v>22.526738999999999</v>
       </c>
-      <c r="I18" s="15">
+      <c r="J18" s="15">
         <f t="shared" si="1"/>
         <v>30.073261000000002</v>
       </c>
-      <c r="J18" s="15">
+      <c r="K18" s="15">
         <f t="shared" si="2"/>
         <v>22.526738999999999</v>
       </c>
-      <c r="K18" s="15">
+      <c r="L18" s="15">
         <f t="shared" si="3"/>
         <v>30.073261000000002</v>
       </c>
-      <c r="L18" s="15">
+      <c r="M18" s="15">
         <f t="shared" si="4"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="M18" s="15">
+      <c r="N18" s="15">
         <f t="shared" si="5"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="N18" s="18">
-        <f>PI()*(L18/2)*H18</f>
-        <v>121.23297825898662</v>
-      </c>
-      <c r="O18" s="21">
-        <f>PI()*(M18/2)*I18</f>
-        <v>216.06537056040165</v>
-      </c>
-      <c r="P18" s="4">
-        <f t="shared" si="15"/>
-        <v>94.832392301415027</v>
-      </c>
-      <c r="Q18" s="18">
+      <c r="O18" s="18">
+        <f>PI()*(M18/2)*(M18/2)*I18</f>
+        <v>207.67936573633961</v>
+      </c>
+      <c r="P18" s="21">
+        <f>PI()*(N18/2)*(N18/2)*J18</f>
+        <v>494.12853854940488</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="17"/>
+        <v>286.44917281306527</v>
+      </c>
+      <c r="R18" s="18">
         <v>1740.9729620603189</v>
       </c>
-      <c r="R18" s="21">
+      <c r="S18" s="21">
         <v>4246.664453844498</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
@@ -1989,59 +2767,63 @@
       <c r="D19" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="5">
+        <f>B19*C19*D19</f>
+        <v>94.248000000000005</v>
+      </c>
+      <c r="F19" s="4">
         <v>11.20337533511975</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>4.4655576300813964</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>2.9627387912564651</v>
       </c>
-      <c r="H19" s="14">
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>8.7366060000000001</v>
       </c>
-      <c r="I19" s="14">
+      <c r="J19" s="14">
         <f t="shared" si="1"/>
         <v>11.663393999999998</v>
       </c>
-      <c r="J19" s="14">
+      <c r="K19" s="14">
         <f t="shared" si="2"/>
         <v>3.5974260000000005</v>
       </c>
-      <c r="K19" s="14">
+      <c r="L19" s="14">
         <f t="shared" si="3"/>
         <v>4.8025739999999999</v>
       </c>
-      <c r="L19" s="14">
+      <c r="M19" s="14">
         <f t="shared" si="4"/>
         <v>1.8843660000000002</v>
       </c>
-      <c r="M19" s="14">
+      <c r="N19" s="14">
         <f t="shared" si="5"/>
         <v>2.5156340000000004</v>
       </c>
-      <c r="N19" s="18">
-        <f>H19*J19*L19</f>
+      <c r="O19" s="18">
+        <f>I19*K19*M19</f>
         <v>59.224292218926792</v>
       </c>
-      <c r="O19" s="21">
-        <f>I19*K19*M19</f>
+      <c r="P19" s="21">
+        <f>J19*L19*N19</f>
         <v>140.91150970633242</v>
       </c>
-      <c r="P19" s="4">
-        <f t="shared" si="15"/>
+      <c r="Q19" s="4">
+        <f t="shared" si="17"/>
         <v>81.687217487405633</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="R19" s="18">
         <v>59.185233310768908</v>
       </c>
-      <c r="R19" s="21">
+      <c r="S19" s="21">
         <v>140.87028058020454</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2054,59 +2836,63 @@
       <c r="D20" s="7">
         <v>6.2</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="16">
+        <f>(1/3)*PI()*(D20/4)*D20*C20</f>
+        <v>101.64204151669296</v>
+      </c>
+      <c r="F20" s="4">
         <v>11.387614634391195</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>11.385112046279241</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>6.3717571242685223</v>
       </c>
-      <c r="H20" s="14">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>8.6509529999999994</v>
       </c>
-      <c r="I20" s="14">
+      <c r="J20" s="14">
         <f t="shared" si="1"/>
         <v>11.549047</v>
       </c>
-      <c r="J20" s="14">
+      <c r="K20" s="14">
         <f t="shared" si="2"/>
         <v>8.6509529999999994</v>
       </c>
-      <c r="K20" s="14">
+      <c r="L20" s="14">
         <f t="shared" si="3"/>
         <v>11.549047</v>
       </c>
-      <c r="L20" s="14">
+      <c r="M20" s="14">
         <f t="shared" si="4"/>
         <v>5.310486</v>
       </c>
-      <c r="M20" s="14">
+      <c r="N20" s="14">
         <f t="shared" si="5"/>
         <v>7.0895140000000003</v>
       </c>
-      <c r="N20" s="18">
-        <f>PI()*(L20/2)*(L20/2)*(J20/3)</f>
+      <c r="O20" s="18">
+        <f>PI()*(M20/2)*(M20/2)*(K20/3)</f>
         <v>63.87061761005976</v>
       </c>
-      <c r="O20" s="21">
-        <f>PI()*(M20/2)*(M20/2)*(K20/3)</f>
+      <c r="P20" s="21">
+        <f>PI()*(N20/2)*(N20/2)*(L20/3)</f>
         <v>151.96644512086121</v>
       </c>
-      <c r="P20" s="4">
-        <f t="shared" si="15"/>
+      <c r="Q20" s="4">
+        <f t="shared" si="17"/>
         <v>88.095827510801456</v>
       </c>
-      <c r="Q20" s="18">
+      <c r="R20" s="18">
         <v>397.44365784226954</v>
       </c>
-      <c r="R20" s="21">
+      <c r="S20" s="21">
         <v>945.57363004341983</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>80</v>
       </c>
@@ -2119,59 +2905,63 @@
       <c r="D21" s="16">
         <v>4.3</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="7">
+        <f>(4/3)*PI()*B21*C21*D22*(1/8)</f>
+        <v>38.725365443250176</v>
+      </c>
+      <c r="F21" s="4">
         <v>4.8587205545333969</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>4.836688740788178</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>4.8675469075455986</v>
       </c>
-      <c r="H21" s="14">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="I21" s="14">
+      <c r="J21" s="14">
         <f t="shared" si="1"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="J21" s="14">
+      <c r="K21" s="14">
         <f t="shared" si="2"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="K21" s="14">
+      <c r="L21" s="14">
         <f t="shared" si="3"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="L21" s="14">
+      <c r="M21" s="14">
         <f t="shared" si="4"/>
         <v>3.6830789999999998</v>
       </c>
-      <c r="M21" s="14">
+      <c r="N21" s="14">
         <f t="shared" si="5"/>
         <v>4.9169209999999994</v>
       </c>
-      <c r="N21" s="18">
-        <f>(4/3)*(H21/2)*(H21/2)*(H21/2)*PI()</f>
+      <c r="O21" s="18">
+        <f>(4/3)*(I21/2)*(I21/2)*(I21/2)*PI()</f>
         <v>26.159637724333255</v>
       </c>
-      <c r="O21" s="21">
-        <f>(4/3)*PI()*(I21/2)*(I21/2)*(I21/2)</f>
+      <c r="P21" s="21">
+        <f>(4/3)*PI()*(J21/2)*(J21/2)*(J21/2)</f>
         <v>62.241251131887708</v>
       </c>
-      <c r="P21" s="4">
-        <f t="shared" si="15"/>
+      <c r="Q21" s="4">
+        <f t="shared" si="17"/>
         <v>36.081613407554457</v>
       </c>
-      <c r="Q21" s="18">
+      <c r="R21" s="18">
         <v>49.965771271225705</v>
       </c>
-      <c r="R21" s="21">
+      <c r="S21" s="21">
         <v>118.87115491800894</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>79</v>
       </c>
@@ -2184,89 +2974,106 @@
       <c r="D22" s="6">
         <v>4</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
+        <f>PI()*D22*D22*(1/4)*B22</f>
+        <v>387.04421492226254</v>
+      </c>
+      <c r="F22" s="6">
         <v>32.435533478011365</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>32.508213569188591</v>
       </c>
-      <c r="G22" s="6">
+      <c r="H22" s="6">
         <v>7.375795168481555</v>
       </c>
-      <c r="H22" s="15">
+      <c r="I22" s="15">
         <f t="shared" si="0"/>
         <v>26.381124</v>
       </c>
-      <c r="I22" s="15">
+      <c r="J22" s="15">
         <f t="shared" si="1"/>
         <v>35.218876000000002</v>
       </c>
-      <c r="J22" s="15">
+      <c r="K22" s="15">
         <f t="shared" si="2"/>
         <v>26.381124</v>
       </c>
-      <c r="K22" s="15">
+      <c r="L22" s="15">
         <f t="shared" si="3"/>
         <v>35.218876000000002</v>
       </c>
-      <c r="L22" s="15">
+      <c r="M22" s="15">
         <f t="shared" si="4"/>
         <v>3.4261200000000001</v>
       </c>
-      <c r="M22" s="15">
+      <c r="N22" s="15">
         <f t="shared" si="5"/>
         <v>4.5738799999999999</v>
       </c>
-      <c r="N22" s="18">
-        <f>PI()*(L22/2)*H22</f>
-        <v>141.97626351242539</v>
-      </c>
-      <c r="O22" s="21">
-        <f>PI()*(M22/2)*I22</f>
-        <v>253.03473054221939</v>
-      </c>
-      <c r="P22" s="4">
-        <f t="shared" si="15"/>
-        <v>111.058467029794</v>
-      </c>
-      <c r="Q22" s="18">
+      <c r="O22" s="18">
+        <f>PI()*(M22/2)*(M22/2)*I22</f>
+        <v>243.21385797259543</v>
+      </c>
+      <c r="P22" s="21">
+        <f>PI()*(N22/2)*(N22/2)*J22</f>
+        <v>578.67524666622319</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="17"/>
+        <v>335.46138869362778</v>
+      </c>
+      <c r="R22" s="18">
         <v>2418.4399470457129</v>
       </c>
-      <c r="R22" s="21">
+      <c r="S22" s="21">
         <v>6060.1004174180453</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
         <v>1</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="4"/>
+      <c r="F24" s="14">
         <f>D24-(D24*0.14347)</f>
         <v>0.85653000000000001</v>
       </c>
-      <c r="F24" s="14">
+      <c r="G24" s="14">
         <f>D24+(D24*0.14347)</f>
         <v>1.14347</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E25" s="4">
-        <f>(F24-E24)</f>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F25" s="4">
+        <f>(G24-F24)</f>
         <v>0.28693999999999997</v>
       </c>
-      <c r="F25" s="4">
-        <f>E25/2</f>
+      <c r="G25" s="4">
+        <f>F25/2</f>
         <v>0.14346999999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M22" xr:uid="{FFACE220-7952-43B2-96AE-1F4FC26979F5}"/>
+  <autoFilter ref="A1:N22" xr:uid="{FFACE220-7952-43B2-96AE-1F4FC26979F5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7E21BC-272C-4049-B93E-ABC7FDFE9A16}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6551C9F9-C83E-43DE-A5A4-87FFF708AB6C}">
   <dimension ref="A1:R10"/>
   <sheetViews>
@@ -2274,23 +3081,23 @@
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
@@ -2346,7 +3153,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -2402,7 +3209,7 @@
         <v>591.00014847088778</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>77</v>
       </c>
@@ -2458,7 +3265,7 @@
         <v>198.32782964828547</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>78</v>
       </c>
@@ -2514,7 +3321,7 @@
         <v>780.45544395645709</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>78</v>
       </c>
@@ -2570,7 +3377,7 @@
         <v>141.27980430022856</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>77</v>
       </c>
@@ -2626,7 +3433,7 @@
         <v>339.36754737243683</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>77</v>
       </c>
@@ -2682,7 +3489,7 @@
         <v>110.76949453070699</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>77</v>
       </c>
@@ -2738,7 +3545,7 @@
         <v>322.94916024267849</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>78</v>
       </c>
@@ -2794,7 +3601,7 @@
         <v>244.0074120778597</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
@@ -2856,7 +3663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K64"/>
   <sheetViews>
@@ -2864,21 +3671,21 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.6640625" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2910,7 +3717,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2951,7 +3758,7 @@
         <v>0.84394879212038876</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -2984,7 +3791,7 @@
         <v>9.9096477860087628E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -3017,7 +3824,7 @@
         <v>0.20906083002999928</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3050,7 +3857,7 @@
         <v>9.7976271008921645E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -3083,7 +3890,7 @@
         <v>0.10963168346337968</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -3116,7 +3923,7 @@
         <v>8.2206685249437819E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3149,7 +3956,7 @@
         <v>5.1680202346236201E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -3182,7 +3989,7 @@
         <v>5.6326578472788984E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -3215,7 +4022,7 @@
         <v>0.18805061565411299</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -3248,7 +4055,7 @@
         <v>0.13875534088276972</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -3281,7 +4088,7 @@
         <v>0.13463016267916655</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -3314,7 +4121,7 @@
         <v>5.342761673497818E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -3347,7 +4154,7 @@
         <v>0.15250686772282018</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -3380,7 +4187,7 @@
         <v>0.1576159794712377</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -3413,7 +4220,7 @@
         <v>0.24326734119386315</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -3446,7 +4253,7 @@
         <v>0.16813452760725292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -3479,7 +4286,7 @@
         <v>0.16792171233719921</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3512,7 +4319,7 @@
         <v>0.16495111092485804</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
@@ -3545,7 +4352,7 @@
         <v>0.13096904287509215</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -3578,7 +4385,7 @@
         <v>0.29861970236615171</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -3611,7 +4418,7 @@
         <v>0.3500546704664193</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -3644,7 +4451,7 @@
         <v>8.5277210209483451E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -3677,7 +4484,7 @@
         <v>9.083971493854627E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
@@ -3710,7 +4517,7 @@
         <v>4.9909763667864524E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
@@ -3743,7 +4550,7 @@
         <v>0.10076177864633599</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -3776,7 +4583,7 @@
         <v>0.10088914132316625</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3809,7 +4616,7 @@
         <v>0.10604645701710406</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
@@ -3842,7 +4649,7 @@
         <v>-1.4433508536755438E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -3875,7 +4682,7 @@
         <v>7.7712438979113077E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -3908,7 +4715,7 @@
         <v>0.17538679973809712</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -3941,7 +4748,7 @@
         <v>7.7371074602798115E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
@@ -3974,7 +4781,7 @@
         <v>0.13135018532043094</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -4007,7 +4814,7 @@
         <v>9.9851739011069265E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
@@ -4040,7 +4847,7 @@
         <v>0.18858936211548602</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -4073,7 +4880,7 @@
         <v>0.192285569950716</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
@@ -4106,7 +4913,7 @@
         <v>-1.9202347478820932E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -4139,7 +4946,7 @@
         <v>7.050425487296233E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -4172,7 +4979,7 @@
         <v>8.127319786358235E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
@@ -4205,7 +5012,7 @@
         <v>0.12885173945530407</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -4238,7 +5045,7 @@
         <v>0.11013049801869308</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
@@ -4271,7 +5078,7 @@
         <v>0.17183064043882679</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -4304,7 +5111,7 @@
         <v>0.15109364113349275</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
@@ -4337,7 +5144,7 @@
         <v>0.13424763465608502</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -4370,7 +5177,7 @@
         <v>0.13084532476447164</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -4403,7 +5210,7 @@
         <v>0.13019381117238349</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
@@ -4436,7 +5243,7 @@
         <v>0.12209820809839012</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -4469,7 +5276,7 @@
         <v>6.6552619577780706E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>50</v>
       </c>
@@ -4502,7 +5309,7 @@
         <v>0.24608920563350867</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
@@ -4535,7 +5342,7 @@
         <v>4.7085413395270857E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>52</v>
       </c>
@@ -4568,7 +5375,7 @@
         <v>4.8672682465858451E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>53</v>
       </c>
@@ -4601,7 +5408,7 @@
         <v>0.72083162043568905</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -4634,7 +5441,7 @@
         <v>9.8370130894093216E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>55</v>
       </c>
@@ -4667,7 +5474,7 @@
         <v>6.3228007162237185E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>56</v>
       </c>
@@ -4700,7 +5507,7 @@
         <v>0.34669945057112039</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
@@ -4733,7 +5540,7 @@
         <v>0.12748659746447477</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -4766,7 +5573,7 @@
         <v>0.12723881646329124</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>59</v>
       </c>
@@ -4799,7 +5606,7 @@
         <v>2.7702761978793882E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
@@ -4832,7 +5639,7 @@
         <v>0.12993501268218538</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -4865,7 +5672,7 @@
         <v>0.12481133506701819</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>62</v>
       </c>
@@ -4898,7 +5705,7 @@
         <v>0.13198765291758111</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>63</v>
       </c>
@@ -4931,7 +5738,7 @@
         <v>5.3101736299070272E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>64</v>
       </c>
@@ -4964,7 +5771,7 @@
         <v>5.5461479519110068E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>65</v>
       </c>

</xml_diff>